<commit_message>
fix incorrect table headers
</commit_message>
<xml_diff>
--- a/Assign2/Assign2 Spreadsheet and Tables.xlsx
+++ b/Assign2/Assign2 Spreadsheet and Tables.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\angus\Major_Project\COMP_7402\Assign2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8347D39-CEFC-4F51-8290-F0952C1912C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51E61B84-AFC1-4AB1-A900-ADBCE042658D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{8398558B-4466-4E9F-BD9E-FF122C44B66C}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="38">
   <si>
     <t>e</t>
   </si>
@@ -163,6 +163,21 @@
   </si>
   <si>
     <t>P(M=e|C)</t>
+  </si>
+  <si>
+    <t>P(M=t|C)</t>
+  </si>
+  <si>
+    <t>P(M=a|C)</t>
+  </si>
+  <si>
+    <t>P(M=o|C)</t>
+  </si>
+  <si>
+    <t>P(M=i|C)</t>
+  </si>
+  <si>
+    <t>P(M=n|C)</t>
   </si>
 </sst>
 </file>
@@ -8253,7 +8268,7 @@
   <dimension ref="A1:Q29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="U18" sqref="U18"/>
+      <selection activeCell="S8" sqref="S8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8308,19 +8323,19 @@
         <v>32</v>
       </c>
       <c r="M3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="N3" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="O3" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="P3" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="Q3" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">

</xml_diff>